<commit_message>
edit: add budget allocations. Formatting needed.
</commit_message>
<xml_diff>
--- a/docs/data/raw-data/bangaloreCMP2020Projetcs.xlsx
+++ b/docs/data/raw-data/bangaloreCMP2020Projetcs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\00_Git Repos\bangalore-cmp-2020\data\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C8BAC1-BFAC-4E5E-9830-DFB3D74AA27D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA0F87D-100A-4BC6-A276-72219D608C7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="4275" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="284">
   <si>
     <t>id</t>
   </si>
@@ -862,6 +862,21 @@
   </si>
   <si>
     <t>12.907571218947462, 77.70585219785673</t>
+  </si>
+  <si>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>13.013255992883385, 77.76103920899732</t>
+  </si>
+  <si>
+    <t>12.914265937865533, 77.48636936233684</t>
+  </si>
+  <si>
+    <t>12.916671511371238, 77.48251674160508</t>
+  </si>
+  <si>
+    <t>13.018173812026925, 77.55657081141072</t>
   </si>
 </sst>
 </file>
@@ -1179,12 +1194,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F311"/>
+  <dimension ref="A1:G311"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A271" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A245" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C279" sqref="C279"/>
+      <selection pane="bottomLeft" activeCell="E269" sqref="E269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,10 +1207,11 @@
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1212,10 +1228,13 @@
         <v>143</v>
       </c>
       <c r="F1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1225,11 +1244,14 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1239,11 +1261,14 @@
       <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1253,8 +1278,11 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1264,8 +1292,11 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1275,11 +1306,14 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1289,11 +1323,14 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1303,11 +1340,14 @@
       <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1317,11 +1357,14 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1331,11 +1374,14 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1010</v>
       </c>
@@ -1345,11 +1391,14 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -1359,8 +1408,11 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1012</v>
       </c>
@@ -1370,11 +1422,14 @@
       <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1013</v>
       </c>
@@ -1384,11 +1439,14 @@
       <c r="C14" t="s">
         <v>16</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1014</v>
       </c>
@@ -1398,8 +1456,11 @@
       <c r="C15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1015</v>
       </c>
@@ -1409,11 +1470,14 @@
       <c r="C16" t="s">
         <v>18</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1016</v>
       </c>
@@ -1423,8 +1487,11 @@
       <c r="C17" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1017</v>
       </c>
@@ -1434,8 +1501,11 @@
       <c r="C18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1018</v>
       </c>
@@ -1445,8 +1515,11 @@
       <c r="C19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1019</v>
       </c>
@@ -1456,8 +1529,11 @@
       <c r="C20" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1020</v>
       </c>
@@ -1467,8 +1543,11 @@
       <c r="C21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1021</v>
       </c>
@@ -1478,11 +1557,14 @@
       <c r="C22" t="s">
         <v>24</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1022</v>
       </c>
@@ -1492,11 +1574,14 @@
       <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1023</v>
       </c>
@@ -1506,8 +1591,11 @@
       <c r="C24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1024</v>
       </c>
@@ -1517,11 +1605,14 @@
       <c r="C25" t="s">
         <v>27</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1025</v>
       </c>
@@ -1531,11 +1622,14 @@
       <c r="C26" t="s">
         <v>28</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="G26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1026</v>
       </c>
@@ -1545,11 +1639,14 @@
       <c r="C27" t="s">
         <v>29</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27">
+        <v>10</v>
+      </c>
+      <c r="G27" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1027</v>
       </c>
@@ -1559,11 +1656,14 @@
       <c r="C28" t="s">
         <v>30</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28">
+        <v>10</v>
+      </c>
+      <c r="G28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1028</v>
       </c>
@@ -1573,11 +1673,14 @@
       <c r="C29" t="s">
         <v>31</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29">
+        <v>10</v>
+      </c>
+      <c r="G29" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1029</v>
       </c>
@@ -1587,11 +1690,14 @@
       <c r="C30" t="s">
         <v>32</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1030</v>
       </c>
@@ -1601,11 +1707,14 @@
       <c r="C31" t="s">
         <v>33</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31">
+        <v>10</v>
+      </c>
+      <c r="G31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1031</v>
       </c>
@@ -1615,11 +1724,14 @@
       <c r="C32" t="s">
         <v>34</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32">
+        <v>10</v>
+      </c>
+      <c r="G32" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1032</v>
       </c>
@@ -1629,11 +1741,14 @@
       <c r="C33" t="s">
         <v>35</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="G33" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1033</v>
       </c>
@@ -1643,11 +1758,14 @@
       <c r="C34" t="s">
         <v>36</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1034</v>
       </c>
@@ -1657,8 +1775,11 @@
       <c r="C35" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1035</v>
       </c>
@@ -1668,8 +1789,11 @@
       <c r="C36" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1036</v>
       </c>
@@ -1679,8 +1803,11 @@
       <c r="C37" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1037</v>
       </c>
@@ -1690,11 +1817,14 @@
       <c r="C38" t="s">
         <v>40</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1038</v>
       </c>
@@ -1704,8 +1834,11 @@
       <c r="C39" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1039</v>
       </c>
@@ -1715,8 +1848,11 @@
       <c r="C40" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1040</v>
       </c>
@@ -1726,11 +1862,14 @@
       <c r="C41" t="s">
         <v>43</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41">
+        <v>10</v>
+      </c>
+      <c r="G41" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1041</v>
       </c>
@@ -1740,8 +1879,11 @@
       <c r="C42" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1042</v>
       </c>
@@ -1751,8 +1893,11 @@
       <c r="C43" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1043</v>
       </c>
@@ -1762,8 +1907,11 @@
       <c r="C44" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1044</v>
       </c>
@@ -1773,11 +1921,14 @@
       <c r="C45" t="s">
         <v>47</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45">
+        <v>10</v>
+      </c>
+      <c r="G45" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1045</v>
       </c>
@@ -1787,8 +1938,11 @@
       <c r="C46" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1046</v>
       </c>
@@ -1798,11 +1952,14 @@
       <c r="C47" t="s">
         <v>49</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1047</v>
       </c>
@@ -1812,8 +1969,11 @@
       <c r="C48" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1048</v>
       </c>
@@ -1823,8 +1983,11 @@
       <c r="C49" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1049</v>
       </c>
@@ -1834,8 +1997,11 @@
       <c r="C50" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1050</v>
       </c>
@@ -1845,11 +2011,14 @@
       <c r="C51" t="s">
         <v>53</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1051</v>
       </c>
@@ -1859,8 +2028,11 @@
       <c r="C52" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2001</v>
       </c>
@@ -1868,7 +2040,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2002</v>
       </c>
@@ -1876,7 +2048,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2003</v>
       </c>
@@ -1884,7 +2056,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2004</v>
       </c>
@@ -1892,7 +2064,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2005</v>
       </c>
@@ -1900,7 +2072,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2006</v>
       </c>
@@ -1908,7 +2080,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2007</v>
       </c>
@@ -1916,7 +2088,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2008</v>
       </c>
@@ -1924,7 +2096,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2009</v>
       </c>
@@ -1932,7 +2104,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2010</v>
       </c>
@@ -1940,7 +2112,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2011</v>
       </c>
@@ -1948,7 +2120,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2012</v>
       </c>
@@ -2980,7 +3152,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>2141</v>
       </c>
@@ -2988,7 +3160,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>2142</v>
       </c>
@@ -2996,7 +3168,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>2143</v>
       </c>
@@ -3004,7 +3176,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>2144</v>
       </c>
@@ -3012,7 +3184,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>2145</v>
       </c>
@@ -3020,7 +3192,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>2146</v>
       </c>
@@ -3028,7 +3200,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>2147</v>
       </c>
@@ -3036,7 +3208,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>2148</v>
       </c>
@@ -3044,7 +3216,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>2149</v>
       </c>
@@ -3052,7 +3224,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>2150</v>
       </c>
@@ -3060,7 +3232,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>2151</v>
       </c>
@@ -3068,7 +3240,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>2152</v>
       </c>
@@ -3076,7 +3248,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>2153</v>
       </c>
@@ -3084,7 +3256,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>2154</v>
       </c>
@@ -3092,7 +3264,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>2155</v>
       </c>
@@ -3100,7 +3272,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>3001</v>
       </c>
@@ -3116,11 +3288,14 @@
       <c r="E208">
         <v>300</v>
       </c>
-      <c r="F208" t="s">
+      <c r="F208">
+        <v>50</v>
+      </c>
+      <c r="G208" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>3002</v>
       </c>
@@ -3136,11 +3311,14 @@
       <c r="E209">
         <v>250</v>
       </c>
-      <c r="F209" t="s">
+      <c r="F209">
+        <v>50</v>
+      </c>
+      <c r="G209" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>3003</v>
       </c>
@@ -3156,11 +3334,14 @@
       <c r="E210">
         <v>250</v>
       </c>
-      <c r="F210" t="s">
+      <c r="F210">
+        <v>50</v>
+      </c>
+      <c r="G210" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>3004</v>
       </c>
@@ -3176,8 +3357,11 @@
       <c r="E211">
         <v>250</v>
       </c>
-    </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F211">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>3005</v>
       </c>
@@ -3193,8 +3377,11 @@
       <c r="E212">
         <v>300</v>
       </c>
-    </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F212">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>3006</v>
       </c>
@@ -3210,11 +3397,14 @@
       <c r="E213">
         <v>300</v>
       </c>
-      <c r="F213" t="s">
+      <c r="F213">
+        <v>50</v>
+      </c>
+      <c r="G213" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>3007</v>
       </c>
@@ -3230,8 +3420,11 @@
       <c r="E214">
         <v>250</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F214">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>3008</v>
       </c>
@@ -3247,11 +3440,14 @@
       <c r="E215">
         <v>250</v>
       </c>
-      <c r="F215" t="s">
+      <c r="F215">
+        <v>50</v>
+      </c>
+      <c r="G215" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>3009</v>
       </c>
@@ -3267,11 +3463,14 @@
       <c r="E216">
         <v>500</v>
       </c>
-      <c r="F216" t="s">
+      <c r="F216">
+        <v>50</v>
+      </c>
+      <c r="G216" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>3010</v>
       </c>
@@ -3287,11 +3486,14 @@
       <c r="E217">
         <v>300</v>
       </c>
-      <c r="F217" t="s">
+      <c r="F217">
+        <v>50</v>
+      </c>
+      <c r="G217" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>3011</v>
       </c>
@@ -3307,11 +3509,14 @@
       <c r="E218">
         <v>300</v>
       </c>
-      <c r="F218" t="s">
+      <c r="F218">
+        <v>50</v>
+      </c>
+      <c r="G218" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>3012</v>
       </c>
@@ -3327,11 +3532,14 @@
       <c r="E219">
         <v>300</v>
       </c>
-      <c r="F219" t="s">
+      <c r="F219">
+        <v>50</v>
+      </c>
+      <c r="G219" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>3013</v>
       </c>
@@ -3347,11 +3555,14 @@
       <c r="E220">
         <v>500</v>
       </c>
-      <c r="F220" t="s">
+      <c r="F220">
+        <v>50</v>
+      </c>
+      <c r="G220" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>3014</v>
       </c>
@@ -3367,11 +3578,14 @@
       <c r="E221">
         <v>500</v>
       </c>
-      <c r="F221" t="s">
+      <c r="F221">
+        <v>50</v>
+      </c>
+      <c r="G221" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>3015</v>
       </c>
@@ -3387,11 +3601,14 @@
       <c r="E222">
         <v>500</v>
       </c>
-      <c r="F222" t="s">
+      <c r="F222">
+        <v>50</v>
+      </c>
+      <c r="G222" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>3016</v>
       </c>
@@ -3407,8 +3624,11 @@
       <c r="E223">
         <v>300</v>
       </c>
-    </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F223">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>3017</v>
       </c>
@@ -3424,8 +3644,11 @@
       <c r="E224">
         <v>500</v>
       </c>
-    </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F224">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>3018</v>
       </c>
@@ -3441,11 +3664,14 @@
       <c r="E225">
         <v>500</v>
       </c>
-      <c r="F225" t="s">
+      <c r="F225">
+        <v>50</v>
+      </c>
+      <c r="G225" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>3019</v>
       </c>
@@ -3461,11 +3687,14 @@
       <c r="E226">
         <v>300</v>
       </c>
-      <c r="F226" t="s">
+      <c r="F226">
+        <v>50</v>
+      </c>
+      <c r="G226" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>3020</v>
       </c>
@@ -3481,11 +3710,14 @@
       <c r="E227">
         <v>300</v>
       </c>
-      <c r="F227" t="s">
+      <c r="F227">
+        <v>50</v>
+      </c>
+      <c r="G227" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>3021</v>
       </c>
@@ -3501,11 +3733,14 @@
       <c r="E228">
         <v>300</v>
       </c>
-      <c r="F228" t="s">
+      <c r="F228">
+        <v>50</v>
+      </c>
+      <c r="G228" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>3022</v>
       </c>
@@ -3521,11 +3756,14 @@
       <c r="E229">
         <v>500</v>
       </c>
-      <c r="F229" t="s">
+      <c r="F229">
+        <v>50</v>
+      </c>
+      <c r="G229" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>3023</v>
       </c>
@@ -3541,11 +3779,14 @@
       <c r="E230">
         <v>250</v>
       </c>
-      <c r="F230" t="s">
+      <c r="F230">
+        <v>50</v>
+      </c>
+      <c r="G230" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>3024</v>
       </c>
@@ -3561,11 +3802,14 @@
       <c r="E231">
         <v>250</v>
       </c>
-      <c r="F231" t="s">
+      <c r="F231">
+        <v>50</v>
+      </c>
+      <c r="G231" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>3025</v>
       </c>
@@ -3581,11 +3825,14 @@
       <c r="E232">
         <v>250</v>
       </c>
-      <c r="F232" t="s">
+      <c r="F232">
+        <v>50</v>
+      </c>
+      <c r="G232" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>3026</v>
       </c>
@@ -3601,11 +3848,14 @@
       <c r="E233">
         <v>250</v>
       </c>
-      <c r="F233" t="s">
+      <c r="F233">
+        <v>50</v>
+      </c>
+      <c r="G233" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>3027</v>
       </c>
@@ -3621,11 +3871,14 @@
       <c r="E234">
         <v>300</v>
       </c>
-      <c r="F234" t="s">
+      <c r="F234">
+        <v>50</v>
+      </c>
+      <c r="G234" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>3028</v>
       </c>
@@ -3641,11 +3894,14 @@
       <c r="E235">
         <v>150</v>
       </c>
-      <c r="F235" t="s">
+      <c r="F235">
+        <v>50</v>
+      </c>
+      <c r="G235" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>3029</v>
       </c>
@@ -3661,11 +3917,14 @@
       <c r="E236">
         <v>350</v>
       </c>
-      <c r="F236" t="s">
+      <c r="F236">
+        <v>50</v>
+      </c>
+      <c r="G236" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>3030</v>
       </c>
@@ -3681,11 +3940,14 @@
       <c r="E237">
         <v>250</v>
       </c>
-      <c r="F237" t="s">
+      <c r="F237">
+        <v>50</v>
+      </c>
+      <c r="G237" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>3031</v>
       </c>
@@ -3701,11 +3963,14 @@
       <c r="E238">
         <v>300</v>
       </c>
-      <c r="F238" t="s">
+      <c r="F238">
+        <v>50</v>
+      </c>
+      <c r="G238" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>3032</v>
       </c>
@@ -3721,11 +3986,14 @@
       <c r="E239">
         <v>150</v>
       </c>
-      <c r="F239" t="s">
+      <c r="F239">
+        <v>50</v>
+      </c>
+      <c r="G239" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>3033</v>
       </c>
@@ -3741,11 +4009,14 @@
       <c r="E240">
         <v>350</v>
       </c>
-      <c r="F240" t="s">
+      <c r="F240">
+        <v>50</v>
+      </c>
+      <c r="G240" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>3034</v>
       </c>
@@ -3761,11 +4032,14 @@
       <c r="E241">
         <v>350</v>
       </c>
-      <c r="F241" t="s">
+      <c r="F241">
+        <v>50</v>
+      </c>
+      <c r="G241" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>3035</v>
       </c>
@@ -3781,11 +4055,14 @@
       <c r="E242">
         <v>350</v>
       </c>
-      <c r="F242" t="s">
+      <c r="F242">
+        <v>50</v>
+      </c>
+      <c r="G242" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>3036</v>
       </c>
@@ -3801,11 +4078,14 @@
       <c r="E243">
         <v>150</v>
       </c>
-      <c r="F243" t="s">
+      <c r="F243">
+        <v>50</v>
+      </c>
+      <c r="G243" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>3037</v>
       </c>
@@ -3821,11 +4101,14 @@
       <c r="E244">
         <v>150</v>
       </c>
-      <c r="F244" t="s">
+      <c r="F244">
+        <v>50</v>
+      </c>
+      <c r="G244" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>3038</v>
       </c>
@@ -3841,11 +4124,14 @@
       <c r="E245">
         <v>250</v>
       </c>
-      <c r="F245" t="s">
+      <c r="F245">
+        <v>50</v>
+      </c>
+      <c r="G245" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>3039</v>
       </c>
@@ -3861,11 +4147,14 @@
       <c r="E246">
         <v>150</v>
       </c>
-      <c r="F246" t="s">
+      <c r="F246">
+        <v>50</v>
+      </c>
+      <c r="G246" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>3040</v>
       </c>
@@ -3881,8 +4170,11 @@
       <c r="E247">
         <v>250</v>
       </c>
-    </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F247">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>3041</v>
       </c>
@@ -3898,11 +4190,14 @@
       <c r="E248">
         <v>250</v>
       </c>
-      <c r="F248" t="s">
+      <c r="F248">
+        <v>50</v>
+      </c>
+      <c r="G248" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>3042</v>
       </c>
@@ -3918,8 +4213,11 @@
       <c r="E249">
         <v>250</v>
       </c>
-    </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F249">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>3043</v>
       </c>
@@ -3935,11 +4233,14 @@
       <c r="E250">
         <v>250</v>
       </c>
-      <c r="F250" t="s">
+      <c r="F250">
+        <v>50</v>
+      </c>
+      <c r="G250" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>3044</v>
       </c>
@@ -3955,11 +4256,14 @@
       <c r="E251">
         <v>250</v>
       </c>
-      <c r="F251" t="s">
+      <c r="F251">
+        <v>50</v>
+      </c>
+      <c r="G251" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>3045</v>
       </c>
@@ -3975,11 +4279,14 @@
       <c r="E252">
         <v>250</v>
       </c>
-      <c r="F252" t="s">
+      <c r="F252">
+        <v>50</v>
+      </c>
+      <c r="G252" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>3046</v>
       </c>
@@ -3995,11 +4302,14 @@
       <c r="E253">
         <v>250</v>
       </c>
-      <c r="F253" t="s">
+      <c r="F253">
+        <v>50</v>
+      </c>
+      <c r="G253" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>3047</v>
       </c>
@@ -4015,11 +4325,14 @@
       <c r="E254">
         <v>250</v>
       </c>
-      <c r="F254" t="s">
+      <c r="F254">
+        <v>50</v>
+      </c>
+      <c r="G254" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>3048</v>
       </c>
@@ -4035,11 +4348,14 @@
       <c r="E255">
         <v>250</v>
       </c>
-      <c r="F255" t="s">
+      <c r="F255">
+        <v>50</v>
+      </c>
+      <c r="G255" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>3049</v>
       </c>
@@ -4055,8 +4371,11 @@
       <c r="E256">
         <v>250</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F256">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>3050</v>
       </c>
@@ -4072,8 +4391,11 @@
       <c r="E257">
         <v>250</v>
       </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F257">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>3051</v>
       </c>
@@ -4089,11 +4411,14 @@
       <c r="E258">
         <v>250</v>
       </c>
-      <c r="F258" t="s">
+      <c r="F258">
+        <v>50</v>
+      </c>
+      <c r="G258" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>3052</v>
       </c>
@@ -4109,11 +4434,14 @@
       <c r="E259">
         <v>250</v>
       </c>
-      <c r="F259" t="s">
+      <c r="F259">
+        <v>50</v>
+      </c>
+      <c r="G259" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>3053</v>
       </c>
@@ -4126,11 +4454,14 @@
       <c r="E260">
         <v>700</v>
       </c>
-      <c r="F260" t="s">
+      <c r="F260">
+        <v>50</v>
+      </c>
+      <c r="G260" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>3054</v>
       </c>
@@ -4143,11 +4474,14 @@
       <c r="E261">
         <v>150</v>
       </c>
-      <c r="F261" t="s">
+      <c r="F261">
+        <v>50</v>
+      </c>
+      <c r="G261" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>3055</v>
       </c>
@@ -4160,8 +4494,11 @@
       <c r="E262">
         <v>450</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F262">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>3056</v>
       </c>
@@ -4174,11 +4511,14 @@
       <c r="E263">
         <v>100</v>
       </c>
-      <c r="F263" t="s">
+      <c r="F263">
+        <v>50</v>
+      </c>
+      <c r="G263" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>3057</v>
       </c>
@@ -4191,11 +4531,14 @@
       <c r="E264">
         <v>150</v>
       </c>
-      <c r="F264" t="s">
+      <c r="F264">
+        <v>50</v>
+      </c>
+      <c r="G264" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>3058</v>
       </c>
@@ -4208,8 +4551,11 @@
       <c r="E265">
         <v>200</v>
       </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F265">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>4001</v>
       </c>
@@ -4219,11 +4565,11 @@
       <c r="C266" t="s">
         <v>199</v>
       </c>
-      <c r="F266" t="s">
+      <c r="G266" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>4002</v>
       </c>
@@ -4233,11 +4579,11 @@
       <c r="C267" t="s">
         <v>200</v>
       </c>
-      <c r="F267" t="s">
+      <c r="G267" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>4003</v>
       </c>
@@ -4247,11 +4593,11 @@
       <c r="C268" t="s">
         <v>201</v>
       </c>
-      <c r="F268" t="s">
+      <c r="G268" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>4004</v>
       </c>
@@ -4261,11 +4607,11 @@
       <c r="C269" t="s">
         <v>202</v>
       </c>
-      <c r="F269" t="s">
+      <c r="G269" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>4005</v>
       </c>
@@ -4275,11 +4621,11 @@
       <c r="C270" t="s">
         <v>203</v>
       </c>
-      <c r="F270" t="s">
+      <c r="G270" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>4006</v>
       </c>
@@ -4289,11 +4635,11 @@
       <c r="C271" t="s">
         <v>204</v>
       </c>
-      <c r="F271" t="s">
+      <c r="G271" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>4007</v>
       </c>
@@ -4303,11 +4649,11 @@
       <c r="C272" t="s">
         <v>205</v>
       </c>
-      <c r="F272" t="s">
+      <c r="G272" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>4008</v>
       </c>
@@ -4317,11 +4663,11 @@
       <c r="C273" t="s">
         <v>206</v>
       </c>
-      <c r="F273" t="s">
+      <c r="G273" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>4009</v>
       </c>
@@ -4331,11 +4677,11 @@
       <c r="C274" t="s">
         <v>207</v>
       </c>
-      <c r="F274" t="s">
+      <c r="G274" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>4010</v>
       </c>
@@ -4345,11 +4691,11 @@
       <c r="C275" t="s">
         <v>208</v>
       </c>
-      <c r="F275" t="s">
+      <c r="G275" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>4011</v>
       </c>
@@ -4359,11 +4705,11 @@
       <c r="C276" t="s">
         <v>209</v>
       </c>
-      <c r="F276" t="s">
+      <c r="G276" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>4012</v>
       </c>
@@ -4373,11 +4719,11 @@
       <c r="C277" t="s">
         <v>210</v>
       </c>
-      <c r="F277" t="s">
+      <c r="G277" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>4013</v>
       </c>
@@ -4387,11 +4733,11 @@
       <c r="C278" t="s">
         <v>211</v>
       </c>
-      <c r="F278" t="s">
+      <c r="G278" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>4014</v>
       </c>
@@ -4401,11 +4747,11 @@
       <c r="C279" t="s">
         <v>212</v>
       </c>
-      <c r="F279" t="s">
+      <c r="G279" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>5001</v>
       </c>
@@ -4418,11 +4764,11 @@
       <c r="D280" t="s">
         <v>229</v>
       </c>
-      <c r="F280" t="s">
+      <c r="G280" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>5002</v>
       </c>
@@ -4435,11 +4781,11 @@
       <c r="D281" t="s">
         <v>231</v>
       </c>
-      <c r="F281" t="s">
+      <c r="G281" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>5003</v>
       </c>
@@ -4452,11 +4798,11 @@
       <c r="D282" t="s">
         <v>231</v>
       </c>
-      <c r="F282" t="s">
+      <c r="G282" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>5004</v>
       </c>
@@ -4470,7 +4816,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>5005</v>
       </c>
@@ -4484,7 +4830,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>5006</v>
       </c>
@@ -4498,7 +4844,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>5007</v>
       </c>
@@ -4512,7 +4858,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>5008</v>
       </c>
@@ -4526,7 +4872,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>5009</v>
       </c>
@@ -4540,7 +4886,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>5010</v>
       </c>
@@ -4554,7 +4900,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>5011</v>
       </c>
@@ -4568,7 +4914,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>5012</v>
       </c>
@@ -4582,7 +4928,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>5013</v>
       </c>
@@ -4595,11 +4941,11 @@
       <c r="D292" t="s">
         <v>246</v>
       </c>
-      <c r="F292" t="s">
+      <c r="G292" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>5014</v>
       </c>
@@ -4613,7 +4959,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>5015</v>
       </c>
@@ -4627,7 +4973,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>5016</v>
       </c>
@@ -4640,11 +4986,11 @@
       <c r="D295" t="s">
         <v>246</v>
       </c>
-      <c r="F295" t="s">
+      <c r="G295" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>5017</v>
       </c>
@@ -4658,7 +5004,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>5018</v>
       </c>
@@ -4672,7 +5018,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>5019</v>
       </c>
@@ -4686,7 +5032,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>5020</v>
       </c>
@@ -4699,11 +5045,11 @@
       <c r="D299" t="s">
         <v>253</v>
       </c>
-      <c r="F299" t="s">
+      <c r="G299" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>5021</v>
       </c>
@@ -4716,11 +5062,11 @@
       <c r="D300" t="s">
         <v>253</v>
       </c>
-      <c r="F300" t="s">
+      <c r="G300" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>5022</v>
       </c>
@@ -4733,11 +5079,11 @@
       <c r="D301" t="s">
         <v>253</v>
       </c>
-      <c r="F301" t="s">
+      <c r="G301" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>5023</v>
       </c>
@@ -4750,11 +5096,11 @@
       <c r="D302" t="s">
         <v>253</v>
       </c>
-      <c r="F302" t="s">
+      <c r="G302" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>5024</v>
       </c>
@@ -4767,11 +5113,11 @@
       <c r="D303" t="s">
         <v>253</v>
       </c>
-      <c r="F303" t="s">
+      <c r="G303" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>5025</v>
       </c>
@@ -4784,11 +5130,11 @@
       <c r="D304" t="s">
         <v>253</v>
       </c>
-      <c r="F304" t="s">
+      <c r="G304" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>5026</v>
       </c>
@@ -4801,8 +5147,11 @@
       <c r="D305" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G305" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>5027</v>
       </c>
@@ -4816,7 +5165,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>5028</v>
       </c>
@@ -4830,7 +5179,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>5029</v>
       </c>
@@ -4844,7 +5193,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>5030</v>
       </c>
@@ -4857,8 +5206,11 @@
       <c r="D309" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G309" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>5031</v>
       </c>
@@ -4871,8 +5223,11 @@
       <c r="D310" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G310" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>5032</v>
       </c>
@@ -4884,6 +5239,9 @@
       </c>
       <c r="D311" t="s">
         <v>239</v>
+      </c>
+      <c r="G311" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: Start of FOB georef + little progress on analysis
</commit_message>
<xml_diff>
--- a/docs/data/raw-data/bangaloreCMP2020Projetcs.xlsx
+++ b/docs/data/raw-data/bangaloreCMP2020Projetcs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\00_Git Repos\bangalore-cmp-2020\data\raw-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DA5F3F-D045-45FA-AE83-6369E0EA9D2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE573CB-BFFA-4461-8487-FAC501873C63}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="2565" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="585">
   <si>
     <t>id</t>
   </si>
@@ -1735,6 +1735,51 @@
   </si>
   <si>
     <t>12.972002456767228, 77.61051735367967</t>
+  </si>
+  <si>
+    <t>12.9113427641161, 77.57429815729775</t>
+  </si>
+  <si>
+    <t>12.956849275144204, 77.69780775936569</t>
+  </si>
+  <si>
+    <t>12.956051725724723, 77.69312516347807</t>
+  </si>
+  <si>
+    <t>12.954715204970352, 77.68394924104837</t>
+  </si>
+  <si>
+    <t>12.968689864766919, 77.60142424615806</t>
+  </si>
+  <si>
+    <t>12.971840853212232, 77.60689869770343</t>
+  </si>
+  <si>
+    <t>12.925435860659025, 77.67544480391703</t>
+  </si>
+  <si>
+    <t>12.976667691086602, 77.59927032472335</t>
+  </si>
+  <si>
+    <t>12.96948427474764, 77.60245180356293</t>
+  </si>
+  <si>
+    <t>12.976120668809553, 77.60374548748605</t>
+  </si>
+  <si>
+    <t>12.972496575353658, 77.61950174788767</t>
+  </si>
+  <si>
+    <t>12.984022431621492, 77.58660712022653</t>
+  </si>
+  <si>
+    <t>12.984309599120063, 77.59716274729055</t>
+  </si>
+  <si>
+    <t>13.012582723434742, 77.62583797263228</t>
+  </si>
+  <si>
+    <t>13.018204179943318, 77.63655273257056</t>
   </si>
 </sst>
 </file>
@@ -2058,15 +2103,15 @@
   <dimension ref="A1:H391"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A356" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D293" sqref="D293"/>
+      <selection pane="bottomLeft" activeCell="H129" sqref="H129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="163.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
@@ -2911,6 +2956,12 @@
       <c r="D53" t="s">
         <v>315</v>
       </c>
+      <c r="G53">
+        <v>2</v>
+      </c>
+      <c r="H53" t="s">
+        <v>571</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
@@ -2925,6 +2976,12 @@
       <c r="D54" t="s">
         <v>315</v>
       </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
@@ -2939,6 +2996,12 @@
       <c r="D55" t="s">
         <v>315</v>
       </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55" t="s">
+        <v>573</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -2953,6 +3016,9 @@
       <c r="D56" t="s">
         <v>315</v>
       </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
@@ -2967,6 +3033,9 @@
       <c r="D57" t="s">
         <v>315</v>
       </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -2981,6 +3050,9 @@
       <c r="D58" t="s">
         <v>315</v>
       </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
@@ -2995,6 +3067,9 @@
       <c r="D59" t="s">
         <v>315</v>
       </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
@@ -3009,6 +3084,9 @@
       <c r="D60" t="s">
         <v>315</v>
       </c>
+      <c r="G60">
+        <v>2</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
@@ -3023,6 +3101,12 @@
       <c r="D61" t="s">
         <v>358</v>
       </c>
+      <c r="G61">
+        <v>2</v>
+      </c>
+      <c r="H61" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
@@ -3037,6 +3121,9 @@
       <c r="D62" t="s">
         <v>358</v>
       </c>
+      <c r="G62">
+        <v>2</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
@@ -3051,6 +3138,12 @@
       <c r="D63" t="s">
         <v>360</v>
       </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+      <c r="H63" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
@@ -3065,8 +3158,11 @@
       <c r="D64" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2013</v>
       </c>
@@ -3079,8 +3175,14 @@
       <c r="D65" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G65">
+        <v>2</v>
+      </c>
+      <c r="H65" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2014</v>
       </c>
@@ -3093,8 +3195,14 @@
       <c r="D66" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G66">
+        <v>2</v>
+      </c>
+      <c r="H66" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2015</v>
       </c>
@@ -3107,8 +3215,14 @@
       <c r="D67" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G67">
+        <v>2</v>
+      </c>
+      <c r="H67" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2016</v>
       </c>
@@ -3121,8 +3235,14 @@
       <c r="D68" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G68">
+        <v>2</v>
+      </c>
+      <c r="H68" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2017</v>
       </c>
@@ -3135,8 +3255,14 @@
       <c r="D69" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G69">
+        <v>2</v>
+      </c>
+      <c r="H69" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2018</v>
       </c>
@@ -3149,8 +3275,11 @@
       <c r="D70" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2019</v>
       </c>
@@ -3163,8 +3292,14 @@
       <c r="D71" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G71">
+        <v>2</v>
+      </c>
+      <c r="H71" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2020</v>
       </c>
@@ -3177,8 +3312,11 @@
       <c r="D72" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2021</v>
       </c>
@@ -3191,8 +3329,11 @@
       <c r="D73" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2022</v>
       </c>
@@ -3205,8 +3346,11 @@
       <c r="D74" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2023</v>
       </c>
@@ -3219,8 +3363,11 @@
       <c r="D75" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2024</v>
       </c>
@@ -3233,8 +3380,11 @@
       <c r="D76" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2025</v>
       </c>
@@ -3247,8 +3397,11 @@
       <c r="D77" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2026</v>
       </c>
@@ -3261,8 +3414,14 @@
       <c r="D78" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G78">
+        <v>2</v>
+      </c>
+      <c r="H78" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2027</v>
       </c>
@@ -3275,8 +3434,11 @@
       <c r="D79" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2028</v>
       </c>
@@ -3289,8 +3451,11 @@
       <c r="D80" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2029</v>
       </c>
@@ -3303,8 +3468,11 @@
       <c r="D81" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2030</v>
       </c>
@@ -3317,8 +3485,11 @@
       <c r="D82" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2031</v>
       </c>
@@ -3331,8 +3502,11 @@
       <c r="D83" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G83">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2032</v>
       </c>
@@ -3345,8 +3519,11 @@
       <c r="D84" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G84">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2033</v>
       </c>
@@ -3359,8 +3536,11 @@
       <c r="D85" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2034</v>
       </c>
@@ -3373,8 +3553,11 @@
       <c r="D86" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2035</v>
       </c>
@@ -3387,8 +3570,11 @@
       <c r="D87" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G87">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2036</v>
       </c>
@@ -3401,8 +3587,11 @@
       <c r="D88" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2037</v>
       </c>
@@ -3415,8 +3604,11 @@
       <c r="D89" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2038</v>
       </c>
@@ -3429,8 +3621,11 @@
       <c r="D90" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2039</v>
       </c>
@@ -3443,8 +3638,11 @@
       <c r="D91" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G91">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2040</v>
       </c>
@@ -3457,8 +3655,11 @@
       <c r="D92" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2041</v>
       </c>
@@ -3471,8 +3672,11 @@
       <c r="D93" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2042</v>
       </c>
@@ -3485,8 +3689,11 @@
       <c r="D94" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G94">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2043</v>
       </c>
@@ -3499,8 +3706,11 @@
       <c r="D95" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2044</v>
       </c>
@@ -3513,8 +3723,11 @@
       <c r="D96" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2045</v>
       </c>
@@ -3527,8 +3740,11 @@
       <c r="D97" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2046</v>
       </c>
@@ -3541,8 +3757,11 @@
       <c r="D98" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G98">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2047</v>
       </c>
@@ -3555,8 +3774,11 @@
       <c r="D99" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G99">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2048</v>
       </c>
@@ -3569,8 +3791,11 @@
       <c r="D100" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2049</v>
       </c>
@@ -3583,8 +3808,11 @@
       <c r="D101" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2050</v>
       </c>
@@ -3597,8 +3825,11 @@
       <c r="D102" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G102">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2051</v>
       </c>
@@ -3611,8 +3842,11 @@
       <c r="D103" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2052</v>
       </c>
@@ -3625,8 +3859,11 @@
       <c r="D104" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G104">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2053</v>
       </c>
@@ -3639,8 +3876,11 @@
       <c r="D105" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2054</v>
       </c>
@@ -3653,8 +3893,11 @@
       <c r="D106" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G106">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2055</v>
       </c>
@@ -3667,8 +3910,14 @@
       <c r="D107" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G107">
+        <v>2</v>
+      </c>
+      <c r="H107" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2056</v>
       </c>
@@ -3681,8 +3930,14 @@
       <c r="D108" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G108">
+        <v>2</v>
+      </c>
+      <c r="H108" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2057</v>
       </c>
@@ -3695,8 +3950,11 @@
       <c r="D109" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2058</v>
       </c>
@@ -3709,8 +3967,11 @@
       <c r="D110" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G110">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2059</v>
       </c>
@@ -3723,8 +3984,11 @@
       <c r="D111" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2060</v>
       </c>
@@ -3737,8 +4001,11 @@
       <c r="D112" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2061</v>
       </c>
@@ -3751,8 +4018,11 @@
       <c r="D113" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2062</v>
       </c>
@@ -3765,8 +4035,11 @@
       <c r="D114" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2063</v>
       </c>
@@ -3779,8 +4052,11 @@
       <c r="D115" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2064</v>
       </c>
@@ -3793,8 +4069,11 @@
       <c r="D116" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G116">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2065</v>
       </c>
@@ -3807,8 +4086,11 @@
       <c r="D117" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2066</v>
       </c>
@@ -3821,8 +4103,11 @@
       <c r="D118" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2067</v>
       </c>
@@ -3835,8 +4120,11 @@
       <c r="D119" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2068</v>
       </c>
@@ -3849,8 +4137,11 @@
       <c r="D120" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2069</v>
       </c>
@@ -3863,8 +4154,11 @@
       <c r="D121" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2070</v>
       </c>
@@ -3877,8 +4171,11 @@
       <c r="D122" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2071</v>
       </c>
@@ -3891,8 +4188,11 @@
       <c r="D123" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2072</v>
       </c>
@@ -3905,8 +4205,11 @@
       <c r="D124" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2073</v>
       </c>
@@ -3919,8 +4222,11 @@
       <c r="D125" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2074</v>
       </c>
@@ -3933,8 +4239,11 @@
       <c r="D126" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G126">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2075</v>
       </c>
@@ -3947,8 +4256,11 @@
       <c r="D127" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2076</v>
       </c>
@@ -3961,8 +4273,11 @@
       <c r="D128" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2077</v>
       </c>
@@ -3975,8 +4290,11 @@
       <c r="D129" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2078</v>
       </c>
@@ -3989,8 +4307,11 @@
       <c r="D130" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G130">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2079</v>
       </c>
@@ -4003,8 +4324,11 @@
       <c r="D131" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2080</v>
       </c>
@@ -4017,8 +4341,11 @@
       <c r="D132" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2081</v>
       </c>
@@ -4031,8 +4358,11 @@
       <c r="D133" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2082</v>
       </c>
@@ -4045,8 +4375,11 @@
       <c r="D134" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2083</v>
       </c>
@@ -4059,8 +4392,11 @@
       <c r="D135" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2084</v>
       </c>
@@ -4073,8 +4409,11 @@
       <c r="D136" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2085</v>
       </c>
@@ -4087,8 +4426,11 @@
       <c r="D137" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2086</v>
       </c>
@@ -4101,8 +4443,11 @@
       <c r="D138" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G138">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2087</v>
       </c>
@@ -4115,8 +4460,11 @@
       <c r="D139" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2088</v>
       </c>
@@ -4129,8 +4477,11 @@
       <c r="D140" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2089</v>
       </c>
@@ -4143,8 +4494,11 @@
       <c r="D141" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2090</v>
       </c>
@@ -4157,8 +4511,11 @@
       <c r="D142" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2091</v>
       </c>
@@ -4171,8 +4528,11 @@
       <c r="D143" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2092</v>
       </c>
@@ -4185,8 +4545,11 @@
       <c r="D144" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G144">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2093</v>
       </c>
@@ -4199,8 +4562,11 @@
       <c r="D145" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2094</v>
       </c>
@@ -4213,8 +4579,11 @@
       <c r="D146" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2095</v>
       </c>
@@ -4227,8 +4596,11 @@
       <c r="D147" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2096</v>
       </c>
@@ -4241,8 +4613,11 @@
       <c r="D148" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2097</v>
       </c>
@@ -4255,8 +4630,11 @@
       <c r="D149" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2098</v>
       </c>
@@ -4269,8 +4647,11 @@
       <c r="D150" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G150">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2099</v>
       </c>
@@ -4283,8 +4664,11 @@
       <c r="D151" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2100</v>
       </c>
@@ -4297,8 +4681,11 @@
       <c r="D152" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G152">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2101</v>
       </c>
@@ -4311,8 +4698,11 @@
       <c r="D153" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2102</v>
       </c>
@@ -4325,8 +4715,11 @@
       <c r="D154" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2103</v>
       </c>
@@ -4339,8 +4732,11 @@
       <c r="D155" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2104</v>
       </c>
@@ -4353,8 +4749,11 @@
       <c r="D156" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2105</v>
       </c>
@@ -4367,8 +4766,11 @@
       <c r="D157" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2106</v>
       </c>
@@ -4381,8 +4783,11 @@
       <c r="D158" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2107</v>
       </c>
@@ -4395,8 +4800,11 @@
       <c r="D159" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2108</v>
       </c>
@@ -4409,8 +4817,11 @@
       <c r="D160" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>2109</v>
       </c>
@@ -4423,8 +4834,11 @@
       <c r="D161" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2110</v>
       </c>
@@ -4437,8 +4851,11 @@
       <c r="D162" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G162">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2111</v>
       </c>
@@ -4451,8 +4868,11 @@
       <c r="D163" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2112</v>
       </c>
@@ -4465,8 +4885,11 @@
       <c r="D164" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2113</v>
       </c>
@@ -4479,8 +4902,11 @@
       <c r="D165" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2114</v>
       </c>
@@ -4493,8 +4919,11 @@
       <c r="D166" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2115</v>
       </c>
@@ -4507,8 +4936,11 @@
       <c r="D167" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2116</v>
       </c>
@@ -4521,8 +4953,11 @@
       <c r="D168" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G168">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2117</v>
       </c>
@@ -4535,8 +4970,11 @@
       <c r="D169" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2118</v>
       </c>
@@ -4549,8 +4987,11 @@
       <c r="D170" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2119</v>
       </c>
@@ -4563,8 +5004,11 @@
       <c r="D171" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>2120</v>
       </c>
@@ -4577,8 +5021,11 @@
       <c r="D172" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G172">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2121</v>
       </c>
@@ -4591,8 +5038,11 @@
       <c r="D173" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2122</v>
       </c>
@@ -4605,8 +5055,11 @@
       <c r="D174" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G174">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2123</v>
       </c>
@@ -4619,8 +5072,11 @@
       <c r="D175" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2124</v>
       </c>
@@ -4633,8 +5089,11 @@
       <c r="D176" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G176">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2125</v>
       </c>
@@ -4647,8 +5106,11 @@
       <c r="D177" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2126</v>
       </c>
@@ -4661,8 +5123,11 @@
       <c r="D178" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G178">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2127</v>
       </c>
@@ -4675,8 +5140,11 @@
       <c r="D179" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2128</v>
       </c>
@@ -4689,8 +5157,11 @@
       <c r="D180" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G180">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2129</v>
       </c>
@@ -4703,8 +5174,11 @@
       <c r="D181" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>2130</v>
       </c>
@@ -4717,8 +5191,11 @@
       <c r="D182" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G182">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>2131</v>
       </c>
@@ -4731,8 +5208,11 @@
       <c r="D183" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>2132</v>
       </c>
@@ -4745,8 +5225,11 @@
       <c r="D184" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G184">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>2133</v>
       </c>
@@ -4759,8 +5242,11 @@
       <c r="D185" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>2134</v>
       </c>
@@ -4773,8 +5259,11 @@
       <c r="D186" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>2135</v>
       </c>
@@ -4787,8 +5276,11 @@
       <c r="D187" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G187">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>2136</v>
       </c>
@@ -4801,8 +5293,11 @@
       <c r="D188" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G188">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>2137</v>
       </c>
@@ -4815,8 +5310,11 @@
       <c r="D189" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>2138</v>
       </c>
@@ -4829,8 +5327,11 @@
       <c r="D190" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G190">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>2139</v>
       </c>
@@ -4843,8 +5344,11 @@
       <c r="D191" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G191">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>2140</v>
       </c>
@@ -4856,6 +5360,9 @@
       </c>
       <c r="D192" t="s">
         <v>453</v>
+      </c>
+      <c r="G192">
+        <v>2</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -4871,6 +5378,9 @@
       <c r="D193" t="s">
         <v>453</v>
       </c>
+      <c r="G193">
+        <v>2</v>
+      </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194">
@@ -4885,6 +5395,9 @@
       <c r="D194" t="s">
         <v>453</v>
       </c>
+      <c r="G194">
+        <v>2</v>
+      </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195">
@@ -4899,6 +5412,9 @@
       <c r="D195" t="s">
         <v>453</v>
       </c>
+      <c r="G195">
+        <v>2</v>
+      </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196">
@@ -4913,6 +5429,9 @@
       <c r="D196" t="s">
         <v>453</v>
       </c>
+      <c r="G196">
+        <v>2</v>
+      </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197">
@@ -4927,6 +5446,9 @@
       <c r="D197" t="s">
         <v>453</v>
       </c>
+      <c r="G197">
+        <v>2</v>
+      </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198">
@@ -4941,6 +5463,9 @@
       <c r="D198" t="s">
         <v>453</v>
       </c>
+      <c r="G198">
+        <v>2</v>
+      </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199">
@@ -5093,6 +5618,9 @@
       </c>
       <c r="G210">
         <v>50</v>
+      </c>
+      <c r="H210" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>